<commit_message>
completed offer detail views and added related buttons
</commit_message>
<xml_diff>
--- a/offer_detail.xlsx
+++ b/offer_detail.xlsx
@@ -500,7 +500,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mal zemesi</t>
+          <t>fas</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -513,7 +513,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kokil</t>
+          <t>sff</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kum</t>
+          <t>sf</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>250</v>
+        <v>3</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TL</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C13" t="inlineStr"/>
     </row>
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C14" t="inlineStr"/>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -629,7 +629,7 @@
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -640,7 +640,7 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -651,7 +651,7 @@
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -662,7 +662,7 @@
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -673,7 +673,7 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -684,7 +684,7 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -695,7 +695,7 @@
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -706,7 +706,7 @@
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -728,7 +728,7 @@
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
details has been created
</commit_message>
<xml_diff>
--- a/offer_detail.xlsx
+++ b/offer_detail.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,11 +439,6 @@
           <t>#</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -456,11 +451,6 @@
           <t>Tekzen</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Tekzen</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -473,11 +463,6 @@
           <t>565333_TEK</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>565333_TEK</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -490,7 +475,6 @@
           <t>Dil Maşası</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -500,10 +484,9 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>fas</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
+          <t>O_O</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -513,10 +496,9 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>sff</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>o_o</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -526,10 +508,9 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>sf</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
+          <t>bruh</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -538,9 +519,8 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -549,9 +529,8 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -560,9 +539,8 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" t="inlineStr"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -571,9 +549,8 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
+        <v>656</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -583,10 +560,9 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+          <t>TL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -595,9 +571,8 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -606,129 +581,339 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6</v>
-      </c>
-      <c r="C14" t="inlineStr"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Kum Döküm</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>0</v>
+          <t>Teslim Türü</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Kokil Döküm</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>0</v>
+          <t>Kalıp Göz Sayısı</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5656</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Enjeksiyon Döküm</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="n">
-        <v>0</v>
+          <t>Maça Göz Sayısı</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Soğuk Maça</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="n">
-        <v>0</v>
+          <t>Kalıp Ömrü Baskı Sayısı</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Takalama</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="n">
-        <v>0</v>
+          <t>Kum Döküm</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Testere</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="n">
-        <v>0</v>
+          <t>Kokil Döküm</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Zımpara</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>0</v>
+          <t>Enjeksiyon Döküm</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>675</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Tesviye</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="n">
-        <v>0</v>
+          <t>Sıcak Maça</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Kumlama</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="n">
-        <v>0</v>
+          <t>Soğuk Maça</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>798</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Test (Sızdırmazlık)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="n">
-        <v>0</v>
+          <t>Takalama</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>657</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
+          <t>Testere</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Zımpara</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Tesviye</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Kumlama</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Test (Sızdırmazlık)</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
           <t>Test (Temizleme)</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
+      <c r="B30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Isıl İşlem (kg bazında hesaplama için)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>Isıl İşlem (şarf bazında hesaplama için)</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Vibrasyon</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>CNC (Dik İşleme)</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>CNC Yatay İşleme</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Torna</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>Heli-Coil</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Montaj (Parça)</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Montaj (Kaynak)</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Paketleme</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>Emprenye</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Kaplama</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>Boya</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Dış İşleme</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>X-Ray Testi</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Mukavemet Testi</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>Nakliye Maliyeti</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added searching bar using Q object
</commit_message>
<xml_diff>
--- a/offer_detail.xlsx
+++ b/offer_detail.xlsx
@@ -448,7 +448,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tekzen</t>
+          <t>Petros Petropoulos</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>565333_TEK</t>
+          <t>69</t>
         </is>
       </c>
     </row>
@@ -472,7 +472,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dil Maşası</t>
+          <t>R_SWING (2)</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>O_O</t>
+          <t>jlj</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>o_o</t>
+          <t>jlkj</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>bruh</t>
+          <t>jlkj</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>65</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>656</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>56</v>
+        <v>565</v>
       </c>
     </row>
     <row r="15">
@@ -592,7 +592,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>dfdf</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5656</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>56</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>56</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>675</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>9</v>
+        <v>979</v>
       </c>
     </row>
     <row r="23">
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>798</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>657</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25">
@@ -693,7 +693,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26">
@@ -703,7 +703,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>57</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -713,7 +713,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28">
@@ -723,7 +723,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>85</v>
+        <v>675</v>
       </c>
     </row>
     <row r="29">
@@ -733,7 +733,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30">
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>765</v>
       </c>
     </row>
     <row r="31">
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>765</v>
+        <v>654</v>
       </c>
     </row>
     <row r="33">
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34">
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>765</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>765</v>
+        <v>6785</v>
       </c>
     </row>
     <row r="36">
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37">
@@ -813,7 +813,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>765</v>
+        <v>687</v>
       </c>
     </row>
     <row r="38">
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>765</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39">
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>875</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40">
@@ -843,7 +843,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41">
@@ -853,7 +853,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>857</v>
       </c>
     </row>
     <row r="42">
@@ -863,7 +863,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>884</v>
+        <v>686</v>
       </c>
     </row>
     <row r="43">
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
@@ -883,7 +883,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>7</v>
+        <v>657</v>
       </c>
     </row>
     <row r="45">
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>465</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46">
@@ -903,7 +903,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
@@ -913,7 +913,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>58</v>
+        <v>568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some searching bars and views
</commit_message>
<xml_diff>
--- a/offer_detail.xlsx
+++ b/offer_detail.xlsx
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>pp00065</t>
         </is>
       </c>
     </row>
@@ -472,7 +472,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R_SWING (2)</t>
+          <t>3lü Priz</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>jlj</t>
+          <t>Kum</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>jlkj</t>
+          <t>Dökmelik</t>
         </is>
       </c>
     </row>
@@ -506,11 +506,7 @@
           <t>Maça Tipi</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>jlkj</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -529,7 +525,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
@@ -539,7 +535,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -549,7 +545,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -571,7 +567,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -581,7 +577,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>565</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15">
@@ -592,7 +588,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>dfdf</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -603,7 +599,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17">
@@ -613,7 +609,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
@@ -623,7 +619,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -633,7 +629,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -643,7 +639,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -653,7 +649,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>68</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -663,7 +659,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>979</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -673,7 +669,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
@@ -683,7 +679,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -693,7 +689,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -703,7 +699,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -713,7 +709,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -723,7 +719,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -733,7 +729,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -743,7 +739,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>765</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -753,7 +749,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -763,7 +759,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -773,7 +769,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -783,7 +779,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -793,7 +789,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>6785</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -803,7 +799,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -813,7 +809,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>687</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -823,7 +819,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -833,7 +829,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -843,7 +839,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -853,7 +849,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -863,7 +859,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>686</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -873,7 +869,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -883,7 +879,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>657</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -893,7 +889,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -903,7 +899,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -913,7 +909,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>568</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>